<commit_message>
-Changes to the budget
Former-commit-id: e0f652494491b6a29aa3b44c76db47f5ed95c9fa
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Equipment" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="External Funding" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Direct Costs</t>
   </si>
@@ -121,6 +122,9 @@
   <si>
     <t>*Please round numbers to the nearest thousand</t>
   </si>
+  <si>
+    <t>Potential / Existing Funder</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +134,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="[$$-1009]#,##0;[RED]\-[$$-1009]#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -172,6 +176,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -271,10 +282,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -309,6 +316,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -496,7 +507,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -508,7 +519,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -524,13 +535,13 @@
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -566,174 +577,195 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="8" t="n">
         <f aca="false">SUM(Equipment!B22)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="8" t="n">
         <f aca="false">SUM(Equipment!C22)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="8" t="n">
         <f aca="false">SUM(Equipment!D22)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="9" t="n">
+      <c r="E10" s="8" t="n">
         <f aca="false">SUM(Equipment!E22)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="8" t="n">
         <f aca="false">SUM(Equipment!F22)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="8" t="n">
         <f aca="false">SUM(Equipment!G22)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="8" t="n">
         <f aca="false">SUM(Equipment!H22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="11" t="n">
+      <c r="B15" s="10" t="n">
         <f aca="false">SUM(B2,B8,B9,B12,B13,B14)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="11" t="n">
+      <c r="C15" s="10" t="n">
         <f aca="false">SUM(C2,C8,C9,C12,C13,C14)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="D15" s="10" t="n">
         <f aca="false">SUM(D2,D8,D9,D12,D13,D14)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="11" t="n">
+      <c r="E15" s="10" t="n">
         <f aca="false">SUM(E2,E8,E9,E12,E13,E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F15" s="10" t="n">
         <f aca="false">SUM(F2,F8,F9,F12,F13,F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="11" t="n">
+      <c r="G15" s="10" t="n">
         <f aca="false">SUM(G2,G8,G9,G12,G13,G14)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="11" t="n">
+      <c r="H15" s="10" t="n">
         <f aca="false">SUM(H2,H8,H9,H12,H13,H14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="B16" s="8" t="n">
+        <f aca="false">'External Funding'!B22</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <f aca="false">'External Funding'!C22</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <f aca="false">'External Funding'!D22</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <f aca="false">'External Funding'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <f aca="false">'External Funding'!F22</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <f aca="false">'External Funding'!G22</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <f aca="false">'External Funding'!H22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="10" t="n">
         <f aca="false">SUM(B15:B16)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="11" t="n">
+      <c r="C17" s="10" t="n">
         <f aca="false">SUM(C15:C16)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D17" s="10" t="n">
         <f aca="false">SUM(D15:D16)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="11" t="n">
+      <c r="E17" s="10" t="n">
         <f aca="false">SUM(E15:E16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="F17" s="10" t="n">
         <f aca="false">SUM(F15:F16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="11" t="n">
+      <c r="G17" s="10" t="n">
         <f aca="false">SUM(G15:G16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="11" t="n">
+      <c r="H17" s="10" t="n">
         <f aca="false">SUM(H15:H16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -757,12 +789,12 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5612244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -793,248 +825,549 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="16" t="n">
+      <c r="B22" s="15" t="n">
         <f aca="false">SUM(B2:B21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="15" t="n">
         <f aca="false">SUM(C2:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="15" t="n">
         <f aca="false">SUM(D2:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="15" t="n">
         <f aca="false">SUM(E2:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="15" t="n">
         <f aca="false">SUM(F2:F21)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="15" t="n">
         <f aca="false">SUM(G2:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="16" t="n">
+      <c r="H22" s="15" t="n">
         <f aca="false">SUM(H2:H21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B24:H24"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="15" t="n">
+        <f aca="false">SUM(B2:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="15" t="n">
+        <f aca="false">SUM(C2:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <f aca="false">SUM(D2:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="15" t="n">
+        <f aca="false">SUM(E2:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15" t="n">
+        <f aca="false">SUM(F2:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="15" t="n">
+        <f aca="false">SUM(G2:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="15" t="n">
+        <f aca="false">SUM(H2:H21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
-Protected the budget template
Former-commit-id: d44c02eb339efcf3ca3e448c2cbe41d5d1821039
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -274,9 +274,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -302,13 +302,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -483,7 +483,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -495,7 +495,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -531,7 +531,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -633,7 +633,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -691,34 +691,34 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="3" t="n">
         <f aca="false">'External Funding'!B22</f>
         <v>0</v>
       </c>
-      <c r="C16" s="8" t="n">
+      <c r="C16" s="3" t="n">
         <f aca="false">'External Funding'!C22</f>
         <v>0</v>
       </c>
-      <c r="D16" s="8" t="n">
+      <c r="D16" s="3" t="n">
         <f aca="false">'External Funding'!D22</f>
         <v>0</v>
       </c>
-      <c r="E16" s="8" t="n">
+      <c r="E16" s="3" t="n">
         <f aca="false">'External Funding'!E22</f>
         <v>0</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="3" t="n">
         <f aca="false">'External Funding'!F22</f>
         <v>0</v>
       </c>
-      <c r="G16" s="8" t="n">
+      <c r="G16" s="3" t="n">
         <f aca="false">'External Funding'!G22</f>
         <v>0</v>
       </c>
-      <c r="H16" s="8" t="n">
+      <c r="H16" s="3" t="n">
         <f aca="false">'External Funding'!H22</f>
         <v>0</v>
       </c>
@@ -768,6 +768,7 @@
       <c r="H19" s="11"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" password="d7fb" objects="true" scenarios="true"/>
   <mergeCells count="1">
     <mergeCell ref="B19:H19"/>
   </mergeCells>
@@ -789,7 +790,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1090,7 +1091,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
-Updated the FES budget
Former-commit-id: 695b0bbd573d4f69cc5d9de41d6347d9a2384533
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="44" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Direct Costs</t>
   </si>
@@ -53,29 +53,44 @@
     <t>1. Compensation Related</t>
   </si>
   <si>
-    <t>  a. Summer</t>
-  </si>
-  <si>
-    <t>  b. Msc / MA</t>
-  </si>
-  <si>
-    <t>  c. PhD</t>
-  </si>
-  <si>
-    <t>  d. PDF/RA</t>
-  </si>
-  <si>
-    <t>  e. Academic</t>
-  </si>
-  <si>
-    <t>2. Travel and Subsistence</t>
-  </si>
-  <si>
-    <t>3. Equipment and Supplies</t>
+    <t>  1.1 Postdoctoral</t>
+  </si>
+  <si>
+    <t>  1.2 Doctorate</t>
+  </si>
+  <si>
+    <t>  1.3 Masters</t>
+  </si>
+  <si>
+    <t>  1.4 Bachelors</t>
+  </si>
+  <si>
+    <t>  1.5 Research Associates</t>
+  </si>
+  <si>
+    <t>  1.6 Research Technical Support (ie. Technicians)</t>
+  </si>
+  <si>
+    <t>  1.7 Research Admin. Support (Managers, Administrators, Research Assistants, Clerks, etc)</t>
+  </si>
+  <si>
+    <t>  1.8 Professional and Technical Services</t>
+  </si>
+  <si>
+    <t>  1.9 Other Misc. Compensation Expenses, incl. Honoraria</t>
+  </si>
+  <si>
+    <t>2. Recruitment and relocation</t>
+  </si>
+  <si>
+    <t>3. Travel, Subsistence</t>
+  </si>
+  <si>
+    <t>4. Equipment and Supplies</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">3.1 Equipment </t>
+      <t xml:space="preserve">  4.1 Equipment </t>
     </r>
     <r>
       <rPr>
@@ -90,16 +105,19 @@
     </r>
   </si>
   <si>
-    <t>3.2 Supplies</t>
-  </si>
-  <si>
-    <t>4. Computers and Electronic Communications</t>
-  </si>
-  <si>
-    <t>5. Dissemination and Networking</t>
-  </si>
-  <si>
-    <t>6. Services</t>
+    <t>  4.2 Supplies</t>
+  </si>
+  <si>
+    <t>5. Sabbatical</t>
+  </si>
+  <si>
+    <t>6. Computers, Electronic Communications</t>
+  </si>
+  <si>
+    <t>7. Dissemination, Networking</t>
+  </si>
+  <si>
+    <t>8. Services and miscellaneous</t>
   </si>
   <si>
     <t>Total Expenditures</t>
@@ -399,20 +417,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.6275510204082"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,35 +461,35 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="n">
-        <f aca="false">SUM(B3:B7)</f>
+        <f aca="false">SUM(B3:B11)</f>
         <v>0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <f aca="false">SUM(C3:C7)</f>
+        <f aca="false">SUM(C3:C11)</f>
         <v>0</v>
       </c>
       <c r="D2" s="3" t="n">
-        <f aca="false">SUM(D3:D7)</f>
+        <f aca="false">SUM(D3:D11)</f>
         <v>0</v>
       </c>
       <c r="E2" s="3" t="n">
-        <f aca="false">SUM(E3:E7)</f>
+        <f aca="false">SUM(E3:E11)</f>
         <v>0</v>
       </c>
       <c r="F2" s="3" t="n">
-        <f aca="false">SUM(F3:F7)</f>
+        <f aca="false">SUM(F3:F11)</f>
         <v>0</v>
       </c>
       <c r="G2" s="3" t="n">
-        <f aca="false">SUM(G3:G7)</f>
+        <f aca="false">SUM(G3:G11)</f>
         <v>0</v>
       </c>
       <c r="H2" s="3" t="n">
-        <f aca="false">SUM(H3:H7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">SUM(H3:H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -483,7 +501,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -532,7 +550,7 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5"/>
@@ -543,73 +561,31 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="n">
-        <f aca="false">SUM(B10:B11)</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <f aca="false">SUM(C10:C11)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <f aca="false">SUM(D10:D11)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <f aca="false">SUM(E10:E11)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <f aca="false">SUM(F10:F11)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <f aca="false">SUM(G10:G11)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <f aca="false">SUM(H10:H11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="n">
-        <f aca="false">SUM(Equipment!B22)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <f aca="false">SUM(Equipment!C22)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <f aca="false">SUM(Equipment!D22)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="8" t="n">
-        <f aca="false">SUM(Equipment!E22)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="n">
-        <f aca="false">SUM(Equipment!F22)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="n">
-        <f aca="false">SUM(Equipment!G22)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <f aca="false">SUM(Equipment!H22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -621,7 +597,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -646,131 +622,245 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="B14" s="3" t="n">
+        <f aca="false">SUM(B15:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <f aca="false">SUM(C15:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <f aca="false">SUM(D15:D16)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <f aca="false">SUM(E15:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <f aca="false">SUM(F15:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <f aca="false">SUM(G15:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <f aca="false">SUM(H15:H16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="10" t="n">
-        <f aca="false">SUM(B2,B8,B9,B12,B13,B14)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="10" t="n">
-        <f aca="false">SUM(C2,C8,C9,C12,C13,C14)</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="10" t="n">
-        <f aca="false">SUM(D2,D8,D9,D12,D13,D14)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="10" t="n">
-        <f aca="false">SUM(E2,E8,E9,E12,E13,E14)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="10" t="n">
-        <f aca="false">SUM(F2,F8,F9,F12,F13,F14)</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="10" t="n">
-        <f aca="false">SUM(G2,G8,G9,G12,G13,G14)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="10" t="n">
-        <f aca="false">SUM(H2,H8,H9,H12,H13,H14)</f>
+      <c r="B15" s="8" t="n">
+        <f aca="false">SUM(Equipment!B22)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <f aca="false">SUM(Equipment!C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <f aca="false">SUM(Equipment!D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8" t="n">
+        <f aca="false">SUM(Equipment!E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <f aca="false">SUM(Equipment!F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <f aca="false">SUM(Equipment!G22)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <f aca="false">SUM(Equipment!H22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <f aca="false">SUM(B2,B13,B14,B17,B19,B20,B12,B18)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <f aca="false">SUM(C2,C13,C14,C17,C19,C20,C12,C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <f aca="false">SUM(D2,D13,D14,D17,D19,D20,D12,D18)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <f aca="false">SUM(E2,E13,E14,E17,E19,E20,E12,E18)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <f aca="false">SUM(F2,F13,F14,F17,F19,F20,F12,F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="10" t="n">
+        <f aca="false">SUM(G2,G13,G14,G17,G19,G20,G12,G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="10" t="n">
+        <f aca="false">SUM(H2,H13,H14,H17,H19,H20,H12,H18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3" t="n">
         <f aca="false">'External Funding'!B22</f>
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C22" s="3" t="n">
         <f aca="false">'External Funding'!C22</f>
         <v>0</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D22" s="3" t="n">
         <f aca="false">'External Funding'!D22</f>
         <v>0</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E22" s="3" t="n">
         <f aca="false">'External Funding'!E22</f>
         <v>0</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F22" s="3" t="n">
         <f aca="false">'External Funding'!F22</f>
         <v>0</v>
       </c>
-      <c r="G16" s="3" t="n">
+      <c r="G22" s="3" t="n">
         <f aca="false">'External Funding'!G22</f>
         <v>0</v>
       </c>
-      <c r="H16" s="3" t="n">
+      <c r="H22" s="3" t="n">
         <f aca="false">'External Funding'!H22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="10" t="n">
-        <f aca="false">B15-B16</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="10" t="n">
-        <f aca="false">C15-C16</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="10" t="n">
-        <f aca="false">D15-D16</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="10" t="n">
-        <f aca="false">E15-E16</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="10" t="n">
-        <f aca="false">F15-F16</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="10" t="n">
-        <f aca="false">G15-G16</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="10" t="n">
-        <f aca="false">H15-H16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <f aca="false">B21-B22</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <f aca="false">C21-C22</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <f aca="false">D21-D22</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <f aca="false">E21-E22</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <f aca="false">F21-F22</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="10" t="n">
+        <f aca="false">G21-G22</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="10" t="n">
+        <f aca="false">H21-H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" password="d7fb" objects="true" scenarios="true"/>
   <mergeCells count="1">
-    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B25:H25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -789,7 +879,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -801,7 +891,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1027,7 +1117,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B22" s="15" t="n">
         <f aca="false">SUM(B2:B21)</f>
@@ -1060,7 +1150,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1090,7 +1180,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1102,7 +1192,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1328,7 +1418,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B22" s="15" t="n">
         <f aca="false">SUM(B2:B21)</f>
@@ -1361,7 +1451,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>

</xml_diff>

<commit_message>
-Changed the FES Budget Template
Former-commit-id: d0cd6c4f21056ca5a5396bf79278d139cd9173a7
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="44" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="22" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Direct Costs</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>5. Sabbatical</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
   <si>
     <t>6. Computers, Electronic Communications</t>
@@ -271,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,6 +308,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -703,17 +710,31 @@
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="B17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -725,7 +746,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -737,7 +758,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -748,41 +769,41 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="10" t="n">
+      <c r="A21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="11" t="n">
         <f aca="false">SUM(B2,B13,B14,B17,B19,B20,B12,B18)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="11" t="n">
         <f aca="false">SUM(C2,C13,C14,C17,C19,C20,C12,C18)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="D21" s="11" t="n">
         <f aca="false">SUM(D2,D13,D14,D17,D19,D20,D12,D18)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="11" t="n">
         <f aca="false">SUM(E2,E13,E14,E17,E19,E20,E12,E18)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="11" t="n">
         <f aca="false">SUM(F2,F13,F14,F17,F19,F20,F12,F18)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="11" t="n">
         <f aca="false">SUM(G2,G13,G14,G17,G19,G20,G12,G18)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="11" t="n">
         <f aca="false">SUM(H2,H13,H14,H17,H19,H20,H12,H18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">'External Funding'!B22</f>
@@ -814,48 +835,48 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="10" t="n">
+      <c r="A23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="11" t="n">
         <f aca="false">B21-B22</f>
         <v>0</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="11" t="n">
         <f aca="false">C21-C22</f>
         <v>0</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="D23" s="11" t="n">
         <f aca="false">D21-D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="11" t="n">
         <f aca="false">E21-E22</f>
         <v>0</v>
       </c>
-      <c r="F23" s="10" t="n">
+      <c r="F23" s="11" t="n">
         <f aca="false">F21-F22</f>
         <v>0</v>
       </c>
-      <c r="G23" s="10" t="n">
+      <c r="G23" s="11" t="n">
         <f aca="false">G21-G22</f>
         <v>0</v>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="11" t="n">
         <f aca="false">H21-H22</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="B25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" password="d7fb" objects="true" scenarios="true"/>
@@ -891,7 +912,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -916,248 +937,248 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="15" t="n">
+      <c r="A22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="16" t="n">
         <f aca="false">SUM(B2:B21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="16" t="n">
         <f aca="false">SUM(C2:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="16" t="n">
         <f aca="false">SUM(D2:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">SUM(E2:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F22" s="16" t="n">
         <f aca="false">SUM(F2:F21)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="15" t="n">
+      <c r="G22" s="16" t="n">
         <f aca="false">SUM(G2:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="15" t="n">
+      <c r="H22" s="16" t="n">
         <f aca="false">SUM(H2:H21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1191,8 +1212,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>34</v>
+      <c r="A1" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1217,248 +1238,248 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="15" t="n">
+      <c r="A22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="16" t="n">
         <f aca="false">SUM(B2:B21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="n">
+      <c r="C22" s="16" t="n">
         <f aca="false">SUM(C2:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="16" t="n">
         <f aca="false">SUM(D2:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">SUM(E2:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F22" s="16" t="n">
         <f aca="false">SUM(F2:F21)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="15" t="n">
+      <c r="G22" s="16" t="n">
         <f aca="false">SUM(G2:G21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="15" t="n">
+      <c r="H22" s="16" t="n">
         <f aca="false">SUM(H2:H21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
-Fixed a problem with creating bibliographies
Former-commit-id: ca1f13eb9be61a40ecfbf8c59413efa7d7acde12
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="22" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="11" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" state="visible" r:id="rId2"/>
@@ -426,13 +426,13 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.4897959183674"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -568,7 +568,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -592,7 +592,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -900,7 +900,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1201,7 +1201,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-Updated the Budget template
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -261,13 +261,13 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -362,12 +362,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,15 +380,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,75 +400,67 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -484,7 +476,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -597,23 +589,23 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="n">
-        <f aca="false">SUM(#REF!)</f>
+        <f aca="false">SUM(C3:C11)</f>
         <v>0</v>
       </c>
       <c r="D2" s="5" t="n">
-        <f aca="false">SUM(#REF!)</f>
+        <f aca="false">SUM(D3:D11)</f>
         <v>0</v>
       </c>
       <c r="E2" s="5" t="n">
-        <f aca="false">SUM(#REF!)</f>
+        <f aca="false">SUM(E3:E11)</f>
         <v>0</v>
       </c>
       <c r="F2" s="5" t="n">
-        <f aca="false">SUM(#REF!)</f>
+        <f aca="false">SUM(F3:F11)</f>
         <v>0</v>
       </c>
       <c r="G2" s="5" t="n">
-        <f aca="false">SUM(#REF!)</f>
+        <f aca="false">SUM(G3:G11)</f>
         <v>0</v>
       </c>
     </row>
@@ -862,60 +854,59 @@
         <f aca="false">G2+G12+G13+G14+G18+G19+G20</f>
         <v>0</v>
       </c>
-      <c r="H21" s="15"/>
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="17" t="n">
+      <c r="C22" s="16" t="n">
         <f aca="false">'External Funding'!C11</f>
         <v>0</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="16" t="n">
         <f aca="false">'External Funding'!D11</f>
         <v>0</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">'External Funding'!E11</f>
         <v>0</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="16" t="n">
         <f aca="false">'External Funding'!F11</f>
         <v>0</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="16" t="n">
         <f aca="false">'External Funding'!G11</f>
         <v>0</v>
       </c>
-      <c r="H22" s="18"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="17" t="n">
+      <c r="C23" s="16" t="n">
         <f aca="false">+'External Funding'!C25</f>
         <v>0</v>
       </c>
-      <c r="D23" s="17" t="n">
+      <c r="D23" s="16" t="n">
         <f aca="false">+'External Funding'!D25</f>
         <v>0</v>
       </c>
-      <c r="E23" s="17" t="n">
+      <c r="E23" s="16" t="n">
         <f aca="false">+'External Funding'!E25</f>
         <v>0</v>
       </c>
-      <c r="F23" s="17" t="n">
+      <c r="F23" s="16" t="n">
         <f aca="false">+'External Funding'!F25</f>
         <v>0</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="16" t="n">
         <f aca="false">+'External Funding'!G25</f>
         <v>0</v>
       </c>
-      <c r="H23" s="18"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="s">
@@ -941,7 +932,7 @@
         <f aca="false">G21+G22+G23</f>
         <v>0</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
       <c r="AMJ24" s="0"/>
     </row>
   </sheetData>
@@ -969,225 +960,225 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="20" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="18" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="25" t="n">
+      <c r="B22" s="23" t="n">
         <f aca="false">SUM(B2:B21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="25" t="n">
+      <c r="C22" s="23" t="n">
         <f aca="false">SUM(C2:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="25" t="n">
+      <c r="D22" s="23" t="n">
         <f aca="false">SUM(D2:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="25" t="n">
+      <c r="E22" s="23" t="n">
         <f aca="false">SUM(E2:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="25" t="n">
+      <c r="F22" s="23" t="n">
         <f aca="false">SUM(F2:F21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1217,268 +1208,268 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="23.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="20" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="23.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="18" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="25" t="n">
+      <c r="C11" s="23" t="n">
         <f aca="false">SUM(C2:C10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="25" t="n">
+      <c r="D11" s="23" t="n">
         <f aca="false">SUM(D2:D10)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="25" t="n">
+      <c r="E11" s="23" t="n">
         <f aca="false">SUM(E2:E10)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="25" t="n">
+      <c r="F11" s="23" t="n">
         <f aca="false">SUM(F2:F10)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="25" t="n">
+      <c r="G11" s="23" t="n">
         <f aca="false">SUM(G2:G10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="25" t="n">
+      <c r="C25" s="23" t="n">
         <f aca="false">SUM(C16:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="25" t="n">
+      <c r="D25" s="23" t="n">
         <f aca="false">SUM(D16:D24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="25" t="n">
+      <c r="E25" s="23" t="n">
         <f aca="false">SUM(E16:E24)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="25" t="n">
+      <c r="F25" s="23" t="n">
         <f aca="false">SUM(F16:F24)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="25" t="n">
+      <c r="G25" s="23" t="n">
         <f aca="false">SUM(G16:G24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
-Changed FES budget template
</commit_message>
<xml_diff>
--- a/data/FES_Project_Budget.xlsx
+++ b/data/FES_Project_Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ferraz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelferraz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E14D0AD-5649-FA42-ABF2-C3E4780BA47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF8271-486C-3D41-A23F-1BBC394B068A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Overall Budget'!$B$1:$F$24</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -118,92 +112,92 @@
 Apr2022 – Mar2023</t>
   </si>
   <si>
+    <t>1. Compensation Related</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.1 Postdoctoral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.2 Doctorate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.3 Masters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.4 Bachelors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.5 Research Associates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.6 Research Technical Support (ie. Technicians)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.7 Research Admin. Support (Managers, Administrators, Research Assistants, Clerks, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.8 Professional and Technical Services</t>
+  </si>
+  <si>
+    <t>3. Travel, Subsistence</t>
+  </si>
+  <si>
+    <t>4. Equipment, Supplies</t>
+  </si>
+  <si>
+    <t>4.1 Equipment (See Equipment worksheet)</t>
+  </si>
+  <si>
+    <t>4.2 Supplies</t>
+  </si>
+  <si>
+    <t>6. Computers, Electronic Communications</t>
+  </si>
+  <si>
+    <t>7. Dissemination, Networking</t>
+  </si>
+  <si>
+    <t>Other Federal Funding</t>
+  </si>
+  <si>
+    <t>External Funding (not Federal)</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>*Please round numbers to the nearest thousand</t>
+  </si>
+  <si>
+    <t>Potential / Existing Funder - Other Federal Funding</t>
+  </si>
+  <si>
+    <t>Potential / Existing Funder - Other Non Federal Funding</t>
+  </si>
+  <si>
+    <t>Request From Future Energy Systems</t>
+  </si>
+  <si>
+    <t>5. Sabbatical</t>
+  </si>
+  <si>
+    <t>2. Recruitment and Relocation</t>
+  </si>
+  <si>
+    <t>8. Services and Miscellaneous</t>
+  </si>
+  <si>
+    <t>Total Funding for the Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.9 Other Compensation Expenses, incl. Honoraria and Research Participation fee</t>
+  </si>
+  <si>
     <t>FY8
-Apr2023 – Sep2023</t>
-  </si>
-  <si>
-    <t>1. Compensation Related</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.1 Postdoctoral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.2 Doctorate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.3 Masters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.4 Bachelors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.5 Research Associates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.6 Research Technical Support (ie. Technicians)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.7 Research Admin. Support (Managers, Administrators, Research Assistants, Clerks, etc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.8 Professional and Technical Services</t>
-  </si>
-  <si>
-    <t>3. Travel, Subsistence</t>
-  </si>
-  <si>
-    <t>4. Equipment, Supplies</t>
-  </si>
-  <si>
-    <t>4.1 Equipment (See Equipment worksheet)</t>
-  </si>
-  <si>
-    <t>4.2 Supplies</t>
-  </si>
-  <si>
-    <t>6. Computers, Electronic Communications</t>
-  </si>
-  <si>
-    <t>7. Dissemination, Networking</t>
-  </si>
-  <si>
-    <t>Other Federal Funding</t>
-  </si>
-  <si>
-    <t>External Funding (not Federal)</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>*Please round numbers to the nearest thousand</t>
-  </si>
-  <si>
-    <t>Potential / Existing Funder - Other Federal Funding</t>
-  </si>
-  <si>
-    <t>Potential / Existing Funder - Other Non Federal Funding</t>
-  </si>
-  <si>
-    <t>Request From Future Energy Systems</t>
-  </si>
-  <si>
-    <t>5. Sabbatical</t>
-  </si>
-  <si>
-    <t>2. Recruitment and Relocation</t>
-  </si>
-  <si>
-    <t>8. Services and Miscellaneous</t>
-  </si>
-  <si>
-    <t>Total Funding for the Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.9 Other Compensation Expenses, incl. Honoraria and Research Participation fee</t>
+Apr2023 – Mar2024</t>
   </si>
 </sst>
 </file>
@@ -918,9 +912,7 @@
   </sheetPr>
   <dimension ref="A1:AMI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="117" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -947,12 +939,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <f>SUM(C3:C11)</f>
@@ -973,7 +965,7 @@
     </row>
     <row r="3" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -982,7 +974,7 @@
     </row>
     <row r="4" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -991,7 +983,7 @@
     </row>
     <row r="5" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1000,7 +992,7 @@
     </row>
     <row r="6" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1009,7 +1001,7 @@
     </row>
     <row r="7" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1018,7 +1010,7 @@
     </row>
     <row r="8" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1027,7 +1019,7 @@
     </row>
     <row r="9" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1036,7 +1028,7 @@
     </row>
     <row r="10" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1045,7 +1037,7 @@
     </row>
     <row r="11" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1054,7 +1046,7 @@
     </row>
     <row r="12" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1063,7 +1055,7 @@
     </row>
     <row r="13" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1072,7 +1064,7 @@
     </row>
     <row r="14" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5">
         <f>C15+C16</f>
@@ -1093,7 +1085,7 @@
     </row>
     <row r="15" spans="2:1023" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="11">
         <f>Equipment!B22</f>
@@ -1115,7 +1107,7 @@
     </row>
     <row r="16" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1124,7 +1116,7 @@
     </row>
     <row r="17" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5">
         <v>0</v>
@@ -1141,7 +1133,7 @@
     </row>
     <row r="18" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1150,7 +1142,7 @@
     </row>
     <row r="19" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1159,7 +1151,7 @@
     </row>
     <row r="20" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1168,7 +1160,7 @@
     </row>
     <row r="21" spans="2:1023" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="14">
         <f>C2+C12+C13+C14+C18+C19+C20</f>
@@ -1190,7 +1182,7 @@
     </row>
     <row r="22" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="16">
         <f>'External Funding'!C11</f>
@@ -1212,7 +1204,7 @@
     </row>
     <row r="23" spans="2:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="16">
         <f>+'External Funding'!C25</f>
@@ -1234,7 +1226,7 @@
     </row>
     <row r="24" spans="2:1023" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="14">
         <f>C21+C22+C23</f>
@@ -1268,7 +1260,7 @@
   <dimension ref="A1:AMH24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1279,7 +1271,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -1291,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1436,7 +1428,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="23">
         <f>SUM(B2:B21)</f>
@@ -1457,7 +1449,7 @@
     </row>
     <row r="23" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -1481,7 +1473,7 @@
   <dimension ref="A1:AMH26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1494,7 +1486,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="57" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>1</v>
@@ -1506,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
@@ -1574,7 +1566,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="23">
         <f>SUM(C2:C10)</f>
@@ -1595,7 +1587,7 @@
     </row>
     <row r="12" spans="2:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -1606,7 +1598,7 @@
     <row r="13" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="2:8" ht="57" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>1</v>
@@ -1618,7 +1610,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
@@ -1686,7 +1678,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="23">
         <f>SUM(C16:C24)</f>
@@ -1707,7 +1699,7 @@
     </row>
     <row r="26" spans="2:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>

</xml_diff>